<commit_message>
Updated Equipment sheet according to the progress
</commit_message>
<xml_diff>
--- a/F78-Gym_equipment/equipments.xlsx
+++ b/F78-Gym_equipment/equipments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Internship\Data_Annotation\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Internship\Data_Annotation\F78-Gym_equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="126">
   <si>
     <t>Original Id</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>Remaining</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -813,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -981,14 +984,14 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3">
         <f>(A7-D7)</f>
@@ -1001,23 +1004,23 @@
         <v>1</v>
       </c>
       <c r="H7" s="4">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3">
         <f>(A8-D8)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1026,23 +1029,23 @@
         <v>1</v>
       </c>
       <c r="H8" s="4">
-        <v>45</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3">
         <f>(A9-D9)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -1051,23 +1054,23 @@
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3">
         <f>(A10-D10)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -1076,19 +1079,19 @@
         <v>1</v>
       </c>
       <c r="H10" s="4">
-        <v>128</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3">
         <f>(A11-D11)</f>
@@ -1101,19 +1104,19 @@
         <v>1</v>
       </c>
       <c r="H11" s="4">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3">
         <f>(A12-D12)</f>
@@ -1126,19 +1129,19 @@
         <v>1</v>
       </c>
       <c r="H12" s="4">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3">
         <f>(A13-D13)</f>
@@ -1151,19 +1154,19 @@
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3">
         <f>(A14-D14)</f>
@@ -1176,19 +1179,19 @@
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
         <f>(A15-D15)</f>
@@ -1201,19 +1204,19 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3">
         <f>(A16-D16)</f>
@@ -1226,19 +1229,19 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E17" s="3">
         <f>(A17-D17)</f>
@@ -1251,19 +1254,19 @@
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3">
         <f>(A18-D18)</f>
@@ -1276,19 +1279,19 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>134</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3">
         <f>(A19-D19)</f>
@@ -1301,19 +1304,19 @@
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20" s="3">
         <f>(A20-D20)</f>
@@ -1326,19 +1329,19 @@
         <v>1</v>
       </c>
       <c r="H20" s="4">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="3">
         <f>(A21-D21)</f>
@@ -1351,19 +1354,19 @@
         <v>1</v>
       </c>
       <c r="H21" s="4">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3">
         <f>(A22-D22)</f>
@@ -1376,19 +1379,19 @@
         <v>1</v>
       </c>
       <c r="H22" s="4">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3">
         <f>(A23-D23)</f>
@@ -1401,19 +1404,19 @@
         <v>1</v>
       </c>
       <c r="H23" s="4">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E24" s="3">
         <f>(A24-D24)</f>
@@ -1426,44 +1429,44 @@
         <v>1</v>
       </c>
       <c r="H24" s="4">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E25" s="3">
         <f>(A25-D25)</f>
         <v>4</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="6">
         <v>1</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
       </c>
       <c r="H25" s="4">
-        <v>122</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E26" s="3">
         <f>(A26-D26)</f>
@@ -1476,19 +1479,19 @@
         <v>1</v>
       </c>
       <c r="H26" s="4">
-        <v>81</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E27" s="3">
         <f>(A27-D27)</f>
@@ -1501,19 +1504,19 @@
         <v>1</v>
       </c>
       <c r="H27" s="4">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E28" s="3">
         <f>(A28-D28)</f>
@@ -1526,19 +1529,19 @@
         <v>1</v>
       </c>
       <c r="H28" s="4">
-        <v>124</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E29" s="3">
         <f>(A29-D29)</f>
@@ -1551,19 +1554,19 @@
         <v>1</v>
       </c>
       <c r="H29" s="4">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E30" s="3">
         <f>(A30-D30)</f>
@@ -1576,19 +1579,19 @@
         <v>1</v>
       </c>
       <c r="H30" s="4">
-        <v>162</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E31" s="3">
         <f>(A31-D31)</f>
@@ -1606,14 +1609,14 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E32" s="3">
         <f>(A32-D32)</f>
@@ -1626,19 +1629,19 @@
         <v>1</v>
       </c>
       <c r="H32" s="4">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E33" s="3">
         <f>(A33-D33)</f>
@@ -1651,19 +1654,19 @@
         <v>1</v>
       </c>
       <c r="H33" s="4">
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E34" s="3">
         <f>(A34-D34)</f>
@@ -1676,19 +1679,19 @@
         <v>1</v>
       </c>
       <c r="H34" s="4">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E35" s="3">
         <f>(A35-D35)</f>
@@ -1701,19 +1704,19 @@
         <v>1</v>
       </c>
       <c r="H35" s="4">
-        <v>129</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E36" s="3">
         <f>(A36-D36)</f>
@@ -1726,19 +1729,19 @@
         <v>1</v>
       </c>
       <c r="H36" s="4">
-        <v>144</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E37" s="3">
         <f>(A37-D37)</f>
@@ -1751,19 +1754,19 @@
         <v>1</v>
       </c>
       <c r="H37" s="4">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E38" s="3">
         <f>(A38-D38)</f>
@@ -1776,19 +1779,19 @@
         <v>1</v>
       </c>
       <c r="H38" s="4">
-        <v>148</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E39" s="3">
         <f>(A39-D39)</f>
@@ -1801,19 +1804,19 @@
         <v>1</v>
       </c>
       <c r="H39" s="4">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E40" s="3">
         <f>(A40-D40)</f>
@@ -1826,19 +1829,19 @@
         <v>1</v>
       </c>
       <c r="H40" s="4">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E41" s="3">
         <f>(A41-D41)</f>
@@ -1851,19 +1854,19 @@
         <v>1</v>
       </c>
       <c r="H41" s="4">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E42" s="3">
         <f>(A42-D42)</f>
@@ -1876,19 +1879,19 @@
         <v>1</v>
       </c>
       <c r="H42" s="4">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E43" s="3">
         <f>(A43-D43)</f>
@@ -1901,19 +1904,19 @@
         <v>1</v>
       </c>
       <c r="H43" s="4">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E44" s="3">
         <f>(A44-D44)</f>
@@ -1926,23 +1929,23 @@
         <v>1</v>
       </c>
       <c r="H44" s="4">
-        <v>172</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E45" s="3">
         <f>(A45-D45)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
@@ -1951,23 +1954,23 @@
         <v>1</v>
       </c>
       <c r="H45" s="4">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E46" s="3">
         <f>(A46-D46)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -1976,23 +1979,23 @@
         <v>1</v>
       </c>
       <c r="H46" s="4">
-        <v>123</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E47" s="3">
         <f>(A47-D47)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -2001,23 +2004,23 @@
         <v>1</v>
       </c>
       <c r="H47" s="4">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E48" s="3">
         <f>(A48-D48)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" s="4">
         <v>1</v>
@@ -2026,23 +2029,23 @@
         <v>1</v>
       </c>
       <c r="H48" s="4">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E49" s="3">
         <f>(A49-D49)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" s="4">
         <v>1</v>
@@ -2051,19 +2054,19 @@
         <v>1</v>
       </c>
       <c r="H49" s="4">
-        <v>194</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E50" s="3">
         <f>(A50-D50)</f>
@@ -2076,19 +2079,19 @@
         <v>1</v>
       </c>
       <c r="H50" s="4">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E51" s="3">
         <f>(A51-D51)</f>
@@ -2101,19 +2104,19 @@
         <v>1</v>
       </c>
       <c r="H51" s="4">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E52" s="3">
         <f>(A52-D52)</f>
@@ -2126,19 +2129,19 @@
         <v>1</v>
       </c>
       <c r="H52" s="4">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E53" s="3">
         <f>(A53-D53)</f>
@@ -2151,19 +2154,19 @@
         <v>1</v>
       </c>
       <c r="H53" s="4">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E54" s="3">
         <f>(A54-D54)</f>
@@ -2176,19 +2179,19 @@
         <v>1</v>
       </c>
       <c r="H54" s="4">
-        <v>110</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E55" s="3">
         <f>(A55-D55)</f>
@@ -2201,19 +2204,19 @@
         <v>1</v>
       </c>
       <c r="H55" s="4">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E56" s="3">
         <f>(A56-D56)</f>
@@ -2226,19 +2229,19 @@
         <v>1</v>
       </c>
       <c r="H56" s="4">
-        <v>212</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E57" s="3">
         <f>(A57-D57)</f>
@@ -2251,19 +2254,19 @@
         <v>1</v>
       </c>
       <c r="H57" s="4">
-        <v>69</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E58" s="3">
         <f>(A58-D58)</f>
@@ -2276,19 +2279,19 @@
         <v>1</v>
       </c>
       <c r="H58" s="4">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E59" s="3">
         <f>(A59-D59)</f>
@@ -2301,19 +2304,19 @@
         <v>1</v>
       </c>
       <c r="H59" s="4">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E60" s="3">
         <f>(A60-D60)</f>
@@ -2326,19 +2329,19 @@
         <v>1</v>
       </c>
       <c r="H60" s="4">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E61" s="3">
         <f>(A61-D61)</f>
@@ -2351,19 +2354,19 @@
         <v>1</v>
       </c>
       <c r="H61" s="4">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E62" s="3">
         <f>(A62-D62)</f>
@@ -2376,19 +2379,19 @@
         <v>1</v>
       </c>
       <c r="H62" s="4">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E63" s="3">
         <f>(A63-D63)</f>
@@ -2401,19 +2404,19 @@
         <v>1</v>
       </c>
       <c r="H63" s="4">
-        <v>157</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E64" s="3">
         <f>(A64-D64)</f>
@@ -2426,19 +2429,19 @@
         <v>1</v>
       </c>
       <c r="H64" s="4">
-        <v>138</v>
+        <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E65" s="3">
         <f>(A65-D65)</f>
@@ -2451,19 +2454,19 @@
         <v>1</v>
       </c>
       <c r="H65" s="4">
-        <v>213</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E66" s="3">
         <f>(A66-D66)</f>
@@ -2476,19 +2479,19 @@
         <v>1</v>
       </c>
       <c r="H66" s="4">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E67" s="3">
         <f>(A67-D67)</f>
@@ -2501,19 +2504,19 @@
         <v>1</v>
       </c>
       <c r="H67" s="4">
-        <v>185</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E68" s="3">
         <f>(A68-D68)</f>
@@ -2526,23 +2529,23 @@
         <v>1</v>
       </c>
       <c r="H68" s="4">
-        <v>155</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E69" s="3">
         <f>(A69-D69)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" s="4">
         <v>1</v>
@@ -2551,23 +2554,23 @@
         <v>1</v>
       </c>
       <c r="H69" s="4">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E70" s="3">
         <f>(A70-D70)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" s="4">
         <v>1</v>
@@ -2576,23 +2579,23 @@
         <v>1</v>
       </c>
       <c r="H70" s="4">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E71" s="3">
         <f>(A71-D71)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F71" s="4">
         <v>1</v>
@@ -2601,23 +2604,23 @@
         <v>1</v>
       </c>
       <c r="H71" s="4">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E72" s="3">
         <f>(A72-D72)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F72" s="4">
         <v>1</v>
@@ -2626,157 +2629,169 @@
         <v>1</v>
       </c>
       <c r="H72" s="4">
-        <v>163</v>
+        <v>48</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="E73" s="3">
         <f>(A73-D73)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
-      <c r="G73" s="4"/>
+      <c r="G73" s="4">
+        <v>1</v>
+      </c>
       <c r="H73" s="4">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="E74" s="3">
         <f>(A74-D74)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F74" s="4">
         <v>1</v>
       </c>
-      <c r="G74" s="4"/>
+      <c r="G74" s="4">
+        <v>1</v>
+      </c>
       <c r="H74" s="4">
-        <v>97</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E75" s="3">
         <f>(A75-D75)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F75" s="4">
         <v>1</v>
       </c>
-      <c r="G75" s="4"/>
+      <c r="G75" s="4">
+        <v>1</v>
+      </c>
       <c r="H75" s="4">
-        <v>80</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="E76" s="3">
         <f>(A76-D76)</f>
-        <v>4</v>
-      </c>
-      <c r="F76" s="6">
-        <v>1</v>
-      </c>
-      <c r="G76" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" s="4">
+        <v>1</v>
+      </c>
       <c r="H76" s="4">
-        <v>77</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="E77" s="3">
         <f>(A77-D77)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F77" s="4">
         <v>1</v>
       </c>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4">
+        <v>1</v>
+      </c>
       <c r="H77" s="4">
-        <v>121</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E78" s="3">
         <f>(A78-D78)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F78" s="4">
         <v>1</v>
       </c>
-      <c r="G78" s="4"/>
+      <c r="G78" s="4">
+        <v>1</v>
+      </c>
       <c r="H78" s="4">
-        <v>133</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="E79" s="3">
         <f>(A79-D79)</f>
@@ -2785,19 +2800,23 @@
       <c r="F79" s="4">
         <v>1</v>
       </c>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+      <c r="G79" s="4">
+        <v>1</v>
+      </c>
+      <c r="H79" s="4">
+        <v>155</v>
+      </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="E80" s="3">
         <f>(A80-D80)</f>
@@ -2806,136 +2825,148 @@
       <c r="F80" s="4">
         <v>1</v>
       </c>
-      <c r="G80" s="4"/>
+      <c r="G80" s="4">
+        <v>1</v>
+      </c>
       <c r="H80" s="4">
-        <v>159</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E81" s="3">
         <f>(A81-D81)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F81" s="4">
         <v>1</v>
       </c>
-      <c r="G81" s="4"/>
+      <c r="G81" s="4">
+        <v>1</v>
+      </c>
       <c r="H81" s="4">
-        <v>190</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E82" s="3">
         <f>(A82-D82)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F82" s="4">
         <v>1</v>
       </c>
-      <c r="G82" s="4"/>
+      <c r="G82" s="4">
+        <v>1</v>
+      </c>
       <c r="H82" s="4">
-        <v>48</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="E83" s="3">
         <f>(A83-D83)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F83" s="4">
         <v>1</v>
       </c>
-      <c r="G83" s="4"/>
+      <c r="G83" s="4">
+        <v>1</v>
+      </c>
       <c r="H83" s="4">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E84" s="3">
         <f>(A84-D84)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F84" s="4">
         <v>1</v>
       </c>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4">
+        <v>1</v>
+      </c>
       <c r="H84" s="4">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E85" s="3">
         <f>(A85-D85)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F85" s="4">
         <v>1</v>
       </c>
-      <c r="G85" s="4"/>
+      <c r="G85" s="4">
+        <v>1</v>
+      </c>
       <c r="H85" s="4">
-        <v>92</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E86" s="3">
         <f>(A86-D86)</f>
@@ -2944,298 +2975,326 @@
       <c r="F86" s="4">
         <v>1</v>
       </c>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4">
+        <v>1</v>
+      </c>
       <c r="H86" s="4">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E87" s="3">
         <f>(A87-D87)</f>
-        <v>1</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>116</v>
+        <v>2</v>
+      </c>
+      <c r="F87" s="4">
+        <v>1</v>
       </c>
       <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
+      <c r="H87" s="4">
+        <v>136</v>
+      </c>
     </row>
     <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E88" s="3">
         <f>(A88-D88)</f>
-        <v>1</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>116</v>
+        <v>3</v>
+      </c>
+      <c r="F88" s="4">
+        <v>1</v>
       </c>
       <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
+      <c r="H88" s="4">
+        <v>73</v>
+      </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E89" s="3">
         <f>(A89-D89)</f>
-        <v>2</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>116</v>
+        <v>3</v>
+      </c>
+      <c r="F89" s="4">
+        <v>1</v>
       </c>
       <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
+      <c r="H89" s="4">
+        <v>174</v>
+      </c>
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E90" s="3">
         <f>(A90-D90)</f>
-        <v>2</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="F90" s="4">
+        <v>1</v>
       </c>
       <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
+      <c r="H90" s="4">
+        <v>86</v>
+      </c>
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E91" s="3">
         <f>(A91-D91)</f>
-        <v>3</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="F91" s="4">
+        <v>1</v>
       </c>
       <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
+      <c r="H91" s="4">
+        <v>121</v>
+      </c>
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E92" s="3">
         <f>(A92-D92)</f>
-        <v>3</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="F92" s="4">
+        <v>1</v>
       </c>
       <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
+      <c r="H92" s="4">
+        <v>119</v>
+      </c>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E93" s="3">
         <f>(A93-D93)</f>
-        <v>3</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F93" s="4">
+        <v>1</v>
       </c>
       <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
+      <c r="H93" s="4">
+        <v>122</v>
+      </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="E94" s="3">
         <f>(A94-D94)</f>
-        <v>3</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F94" s="4">
+        <v>1</v>
       </c>
       <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
+      <c r="H94" s="4">
+        <v>132</v>
+      </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="E95" s="3">
         <f>(A95-D95)</f>
-        <v>4</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F95" s="4">
+        <v>1</v>
       </c>
       <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="4">
+        <v>113</v>
+      </c>
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="E96" s="3">
         <f>(A96-D96)</f>
-        <v>4</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F96" s="4">
+        <v>1</v>
       </c>
       <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
+      <c r="H96" s="4">
+        <v>126</v>
+      </c>
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="E97" s="3">
         <f>(A97-D97)</f>
-        <v>4</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F97" s="4">
+        <v>1</v>
       </c>
       <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
+      <c r="H97" s="4">
+        <v>54</v>
+      </c>
     </row>
     <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="E98" s="3">
         <f>(A98-D98)</f>
-        <v>4</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F98" s="4">
+        <v>1</v>
       </c>
       <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+      <c r="H98" s="4">
+        <v>94</v>
+      </c>
     </row>
     <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="E99" s="3">
         <f>(A99-D99)</f>
-        <v>4</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F99" s="4">
+        <v>1</v>
       </c>
       <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
+      <c r="H99" s="4">
+        <v>97</v>
+      </c>
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E100" s="3">
         <f>(A100-D100)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>116</v>
@@ -3245,18 +3304,18 @@
     </row>
     <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="E101" s="3">
         <f>(A101-D101)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>116</v>
@@ -3266,18 +3325,18 @@
     </row>
     <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="E102" s="3">
         <f>(A102-D102)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>116</v>
@@ -3287,18 +3346,18 @@
     </row>
     <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="E103" s="3">
         <f>(A103-D103)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>116</v>
@@ -3308,18 +3367,18 @@
     </row>
     <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E104" s="3">
         <f>(A104-D104)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>116</v>
@@ -3329,18 +3388,18 @@
     </row>
     <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E105" s="3">
         <f>(A105-D105)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>116</v>
@@ -3350,18 +3409,18 @@
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E106" s="3">
         <f>(A106-D106)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>116</v>
@@ -3371,18 +3430,18 @@
     </row>
     <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="E107" s="3">
         <f>(A107-D107)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>116</v>
@@ -3392,14 +3451,14 @@
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E108" s="3">
         <f>(A108-D108)</f>
@@ -3413,14 +3472,14 @@
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="E109" s="3">
         <f>(A109-D109)</f>
@@ -3434,14 +3493,14 @@
     </row>
     <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E110" s="3">
         <f>(A110-D110)</f>
@@ -3455,14 +3514,14 @@
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E111" s="3">
         <f>(A111-D111)</f>
@@ -3476,26 +3535,24 @@
     </row>
     <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E112" s="3">
         <f>(A112-D112)</f>
-        <v>6</v>
-      </c>
-      <c r="F112" s="3">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="G112" s="4"/>
-      <c r="H112" s="4">
-        <v>155</v>
-      </c>
+      <c r="H112" s="4"/>
     </row>
     <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
@@ -3507,7 +3564,7 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2">
         <f>SUM(F1:F112)</f>
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>121</v>
@@ -3526,15 +3583,15 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2">
         <f>COUNTIF(F1:F112,"a")</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G114" s="1">
         <f>SUM(G1:G112)</f>
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="H114" s="1">
         <f>SUM(H1:H112)</f>
-        <v>10830</v>
+        <v>12249</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3543,7 +3600,7 @@
       </c>
       <c r="F115">
         <f>COUNT(A2:A112)-(F113+F114)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sheet for the equipment updated
</commit_message>
<xml_diff>
--- a/F78-Gym_equipment/equipments.xlsx
+++ b/F78-Gym_equipment/equipments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Original Id</t>
   </si>
@@ -367,9 +367,6 @@
   </si>
   <si>
     <t>Wheel Roller</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Uploaded</t>
@@ -836,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
@@ -849,10 +846,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3459,153 +3456,159 @@
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E106" s="3">
         <f>(A106-D106)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F106" s="3">
         <v>1</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E107" s="3">
         <f>(A107-D107)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F107" s="3">
         <v>1</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4">
-        <v>50</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E108" s="3">
         <f>(A108-D108)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F108" s="3">
         <v>1</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4">
-        <v>134</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="E109" s="3">
         <f>(A109-D109)</f>
-        <v>2</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>116</v>
+        <v>5</v>
+      </c>
+      <c r="F109" s="3">
+        <v>1</v>
       </c>
       <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
+      <c r="H109" s="4">
+        <v>117</v>
+      </c>
     </row>
     <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E110" s="3">
         <f>(A110-D110)</f>
         <v>5</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>116</v>
+      <c r="F110" s="3">
+        <v>1</v>
       </c>
       <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
+      <c r="H110" s="4">
+        <v>134</v>
+      </c>
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="E111" s="3">
         <f>(A111-D111)</f>
-        <v>4</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>125</v>
+        <v>5</v>
+      </c>
+      <c r="F111" s="3">
+        <v>1</v>
       </c>
       <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
+      <c r="H111" s="4">
+        <v>81</v>
+      </c>
     </row>
     <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="E112" s="3">
         <f>(A112-D112)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
@@ -3613,33 +3616,33 @@
     <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2">
         <f>SUM(F1:F112)</f>
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G113" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H113" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2">
         <f>COUNTIF(F1:F112,"a")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G114" s="1">
         <f>SUM(G1:G112)</f>
@@ -3647,16 +3650,16 @@
       </c>
       <c r="H114" s="1">
         <f>SUM(H1:H112)</f>
-        <v>13180</v>
+        <v>13495</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F115">
         <f>COUNT(A2:A112)-(F113+F114)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Script to get some random images to ../Equipment/Preprocessed folder
</commit_message>
<xml_diff>
--- a/F78-Gym_equipment/equipments.xlsx
+++ b/F78-Gym_equipment/equipments.xlsx
@@ -814,7 +814,7 @@
   <dimension ref="A1:H115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H112" sqref="A1:H112"/>
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -981,14 +981,14 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
         <f>(A7-D7)</f>
@@ -1001,19 +1001,19 @@
         <v>1</v>
       </c>
       <c r="H7" s="4">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3">
         <f>(A8-D8)</f>
@@ -1026,23 +1026,23 @@
         <v>1</v>
       </c>
       <c r="H8" s="4">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3">
         <f>(A9-D9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -1051,19 +1051,19 @@
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3">
         <f>(A10-D10)</f>
@@ -1076,19 +1076,19 @@
         <v>1</v>
       </c>
       <c r="H10" s="4">
-        <v>73</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3">
         <f>(A11-D11)</f>
@@ -1101,19 +1101,19 @@
         <v>1</v>
       </c>
       <c r="H11" s="4">
-        <v>139</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3">
         <f>(A12-D12)</f>
@@ -1126,19 +1126,19 @@
         <v>1</v>
       </c>
       <c r="H12" s="4">
-        <v>174</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3">
         <f>(A13-D13)</f>
@@ -1151,19 +1151,19 @@
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <v>156</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3">
         <f>(A14-D14)</f>
@@ -1176,19 +1176,19 @@
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <v>97</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3">
         <f>(A15-D15)</f>
@@ -1201,19 +1201,19 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>80</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="3">
         <f>(A16-D16)</f>
@@ -1226,23 +1226,23 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <v>166</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="3">
         <f>(A17-D17)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -1251,23 +1251,23 @@
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="3">
         <f>(A18-D18)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -1276,19 +1276,19 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>75</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3">
         <f>(A19-D19)</f>
@@ -1301,19 +1301,19 @@
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <v>128</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="3">
         <f>(A20-D20)</f>
@@ -1326,19 +1326,19 @@
         <v>1</v>
       </c>
       <c r="H20" s="4">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="3">
         <f>(A21-D21)</f>
@@ -1351,19 +1351,19 @@
         <v>1</v>
       </c>
       <c r="H21" s="4">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3">
         <f>(A22-D22)</f>
@@ -1376,19 +1376,19 @@
         <v>1</v>
       </c>
       <c r="H22" s="4">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <f>(A23-D23)</f>
@@ -1401,19 +1401,19 @@
         <v>1</v>
       </c>
       <c r="H23" s="4">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3">
         <f>(A24-D24)</f>
@@ -1426,19 +1426,19 @@
         <v>1</v>
       </c>
       <c r="H24" s="4">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3">
         <f>(A25-D25)</f>
@@ -1451,19 +1451,19 @@
         <v>1</v>
       </c>
       <c r="H25" s="4">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E26" s="3">
         <f>(A26-D26)</f>
@@ -1476,19 +1476,19 @@
         <v>1</v>
       </c>
       <c r="H26" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27" s="3">
         <f>(A27-D27)</f>
@@ -1501,19 +1501,19 @@
         <v>1</v>
       </c>
       <c r="H27" s="4">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E28" s="3">
         <f>(A28-D28)</f>
@@ -1526,19 +1526,19 @@
         <v>1</v>
       </c>
       <c r="H28" s="4">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E29" s="3">
         <f>(A29-D29)</f>
@@ -1551,19 +1551,19 @@
         <v>1</v>
       </c>
       <c r="H29" s="4">
-        <v>134</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E30" s="3">
         <f>(A30-D30)</f>
@@ -1576,19 +1576,19 @@
         <v>1</v>
       </c>
       <c r="H30" s="4">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3">
         <f>(A31-D31)</f>
@@ -1601,19 +1601,19 @@
         <v>1</v>
       </c>
       <c r="H31" s="4">
-        <v>111</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3">
         <f>(A32-D32)</f>
@@ -1626,44 +1626,44 @@
         <v>1</v>
       </c>
       <c r="H32" s="4">
-        <v>138</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E33" s="3">
         <f>(A33-D33)</f>
         <v>4</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="4">
         <v>1</v>
       </c>
       <c r="G33" s="4">
         <v>1</v>
       </c>
       <c r="H33" s="4">
-        <v>77</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E34" s="3">
         <f>(A34-D34)</f>
@@ -1676,44 +1676,44 @@
         <v>1</v>
       </c>
       <c r="H34" s="4">
-        <v>113</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" s="3">
         <f>(A35-D35)</f>
         <v>4</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="6">
         <v>1</v>
       </c>
       <c r="G35" s="4">
         <v>1</v>
       </c>
       <c r="H35" s="4">
-        <v>144</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E36" s="3">
         <f>(A36-D36)</f>
@@ -1726,19 +1726,19 @@
         <v>1</v>
       </c>
       <c r="H36" s="4">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E37" s="3">
         <f>(A37-D37)</f>
@@ -1751,19 +1751,19 @@
         <v>1</v>
       </c>
       <c r="H37" s="4">
-        <v>121</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E38" s="3">
         <f>(A38-D38)</f>
@@ -1776,19 +1776,19 @@
         <v>1</v>
       </c>
       <c r="H38" s="4">
-        <v>122</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E39" s="3">
         <f>(A39-D39)</f>
@@ -1801,19 +1801,19 @@
         <v>1</v>
       </c>
       <c r="H39" s="4">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E40" s="3">
         <f>(A40-D40)</f>
@@ -1826,19 +1826,19 @@
         <v>1</v>
       </c>
       <c r="H40" s="4">
-        <v>81</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E41" s="3">
         <f>(A41-D41)</f>
@@ -1851,19 +1851,19 @@
         <v>1</v>
       </c>
       <c r="H41" s="4">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E42" s="3">
         <f>(A42-D42)</f>
@@ -1876,19 +1876,19 @@
         <v>1</v>
       </c>
       <c r="H42" s="4">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E43" s="3">
         <f>(A43-D43)</f>
@@ -1901,19 +1901,19 @@
         <v>1</v>
       </c>
       <c r="H43" s="4">
-        <v>144</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E44" s="3">
         <f>(A44-D44)</f>
@@ -1926,19 +1926,19 @@
         <v>1</v>
       </c>
       <c r="H44" s="4">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E45" s="3">
         <f>(A45-D45)</f>
@@ -1951,19 +1951,19 @@
         <v>1</v>
       </c>
       <c r="H45" s="4">
-        <v>81</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E46" s="3">
         <f>(A46-D46)</f>
@@ -1976,19 +1976,19 @@
         <v>1</v>
       </c>
       <c r="H46" s="4">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E47" s="3">
         <f>(A47-D47)</f>
@@ -2001,19 +2001,19 @@
         <v>1</v>
       </c>
       <c r="H47" s="4">
-        <v>86</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E48" s="3">
         <f>(A48-D48)</f>
@@ -2026,19 +2026,19 @@
         <v>1</v>
       </c>
       <c r="H48" s="4">
-        <v>139</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E49" s="3">
         <f>(A49-D49)</f>
@@ -2051,19 +2051,19 @@
         <v>1</v>
       </c>
       <c r="H49" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E50" s="3">
         <f>(A50-D50)</f>
@@ -2076,19 +2076,19 @@
         <v>1</v>
       </c>
       <c r="H50" s="4">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E51" s="3">
         <f>(A51-D51)</f>
@@ -2101,19 +2101,19 @@
         <v>1</v>
       </c>
       <c r="H51" s="4">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E52" s="3">
         <f>(A52-D52)</f>
@@ -2126,19 +2126,19 @@
         <v>1</v>
       </c>
       <c r="H52" s="4">
-        <v>103</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E53" s="3">
         <f>(A53-D53)</f>
@@ -2151,19 +2151,19 @@
         <v>1</v>
       </c>
       <c r="H53" s="4">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E54" s="3">
         <f>(A54-D54)</f>
@@ -2176,19 +2176,19 @@
         <v>1</v>
       </c>
       <c r="H54" s="4">
-        <v>121</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E55" s="3">
         <f>(A55-D55)</f>
@@ -2201,19 +2201,19 @@
         <v>1</v>
       </c>
       <c r="H55" s="4">
-        <v>161</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E56" s="3">
         <f>(A56-D56)</f>
@@ -2226,19 +2226,19 @@
         <v>1</v>
       </c>
       <c r="H56" s="4">
-        <v>177</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E57" s="3">
         <f>(A57-D57)</f>
@@ -2251,19 +2251,19 @@
         <v>1</v>
       </c>
       <c r="H57" s="4">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E58" s="3">
         <f>(A58-D58)</f>
@@ -2276,19 +2276,19 @@
         <v>1</v>
       </c>
       <c r="H58" s="4">
-        <v>123</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E59" s="3">
         <f>(A59-D59)</f>
@@ -2301,23 +2301,23 @@
         <v>1</v>
       </c>
       <c r="H59" s="4">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3">
         <f>(A60-D60)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" s="4">
         <v>1</v>
@@ -2326,23 +2326,23 @@
         <v>1</v>
       </c>
       <c r="H60" s="4">
-        <v>133</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E61" s="3">
         <f>(A61-D61)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" s="4">
         <v>1</v>
@@ -2356,18 +2356,18 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E62" s="3">
         <f>(A62-D62)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" s="4">
         <v>1</v>
@@ -2376,19 +2376,19 @@
         <v>1</v>
       </c>
       <c r="H62" s="4">
-        <v>123</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E63" s="3">
         <f>(A63-D63)</f>
@@ -2401,19 +2401,19 @@
         <v>1</v>
       </c>
       <c r="H63" s="4">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E64" s="3">
         <f>(A64-D64)</f>
@@ -2426,19 +2426,19 @@
         <v>1</v>
       </c>
       <c r="H64" s="4">
-        <v>194</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E65" s="3">
         <f>(A65-D65)</f>
@@ -2451,19 +2451,19 @@
         <v>1</v>
       </c>
       <c r="H65" s="4">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E66" s="3">
         <f>(A66-D66)</f>
@@ -2476,19 +2476,19 @@
         <v>1</v>
       </c>
       <c r="H66" s="4">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E67" s="3">
         <f>(A67-D67)</f>
@@ -2501,19 +2501,19 @@
         <v>1</v>
       </c>
       <c r="H67" s="4">
-        <v>152</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E68" s="3">
         <f>(A68-D68)</f>
@@ -2526,19 +2526,19 @@
         <v>1</v>
       </c>
       <c r="H68" s="4">
-        <v>122</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E69" s="3">
         <f>(A69-D69)</f>
@@ -2551,19 +2551,19 @@
         <v>1</v>
       </c>
       <c r="H69" s="4">
-        <v>132</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E70" s="3">
         <f>(A70-D70)</f>
@@ -2576,19 +2576,19 @@
         <v>1</v>
       </c>
       <c r="H70" s="4">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E71" s="3">
         <f>(A71-D71)</f>
@@ -2601,19 +2601,19 @@
         <v>1</v>
       </c>
       <c r="H71" s="4">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E72" s="3">
         <f>(A72-D72)</f>
@@ -2626,19 +2626,19 @@
         <v>1</v>
       </c>
       <c r="H72" s="4">
-        <v>93</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E73" s="3">
         <f>(A73-D73)</f>
@@ -2651,19 +2651,19 @@
         <v>1</v>
       </c>
       <c r="H73" s="4">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E74" s="3">
         <f>(A74-D74)</f>
@@ -2676,19 +2676,19 @@
         <v>1</v>
       </c>
       <c r="H74" s="4">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E75" s="3">
         <f>(A75-D75)</f>
@@ -2701,19 +2701,19 @@
         <v>1</v>
       </c>
       <c r="H75" s="4">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E76" s="3">
         <f>(A76-D76)</f>
@@ -2726,19 +2726,19 @@
         <v>1</v>
       </c>
       <c r="H76" s="4">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E77" s="3">
         <f>(A77-D77)</f>
@@ -2751,19 +2751,19 @@
         <v>1</v>
       </c>
       <c r="H77" s="4">
-        <v>190</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E78" s="3">
         <f>(A78-D78)</f>
@@ -2776,19 +2776,19 @@
         <v>1</v>
       </c>
       <c r="H78" s="4">
-        <v>212</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E79" s="3">
         <f>(A79-D79)</f>
@@ -2801,19 +2801,19 @@
         <v>1</v>
       </c>
       <c r="H79" s="4">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E80" s="3">
         <f>(A80-D80)</f>
@@ -2826,19 +2826,19 @@
         <v>1</v>
       </c>
       <c r="H80" s="4">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E81" s="3">
         <f>(A81-D81)</f>
@@ -2856,14 +2856,14 @@
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E82" s="3">
         <f>(A82-D82)</f>
@@ -2876,19 +2876,19 @@
         <v>1</v>
       </c>
       <c r="H82" s="4">
-        <v>121</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E83" s="3">
         <f>(A83-D83)</f>
@@ -2901,19 +2901,19 @@
         <v>1</v>
       </c>
       <c r="H83" s="4">
-        <v>101</v>
+        <v>212</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E84" s="3">
         <f>(A84-D84)</f>
@@ -2926,19 +2926,19 @@
         <v>1</v>
       </c>
       <c r="H84" s="4">
-        <v>128</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E85" s="3">
         <f>(A85-D85)</f>
@@ -2951,19 +2951,19 @@
         <v>1</v>
       </c>
       <c r="H85" s="4">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E86" s="3">
         <f>(A86-D86)</f>
@@ -2976,19 +2976,19 @@
         <v>1</v>
       </c>
       <c r="H86" s="4">
-        <v>157</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E87" s="3">
         <f>(A87-D87)</f>
@@ -3001,19 +3001,19 @@
         <v>1</v>
       </c>
       <c r="H87" s="4">
-        <v>48</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E88" s="3">
         <f>(A88-D88)</f>
@@ -3026,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="H88" s="4">
-        <v>54</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E89" s="3">
         <f>(A89-D89)</f>
@@ -3051,19 +3051,19 @@
         <v>1</v>
       </c>
       <c r="H89" s="4">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E90" s="3">
         <f>(A90-D90)</f>
@@ -3076,19 +3076,19 @@
         <v>1</v>
       </c>
       <c r="H90" s="4">
-        <v>213</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E91" s="3">
         <f>(A91-D91)</f>
@@ -3101,19 +3101,19 @@
         <v>1</v>
       </c>
       <c r="H91" s="4">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E92" s="3">
         <f>(A92-D92)</f>
@@ -3126,19 +3126,19 @@
         <v>1</v>
       </c>
       <c r="H92" s="4">
-        <v>148</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E93" s="3">
         <f>(A93-D93)</f>
@@ -3151,19 +3151,19 @@
         <v>1</v>
       </c>
       <c r="H93" s="4">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E94" s="3">
         <f>(A94-D94)</f>
@@ -3176,19 +3176,19 @@
         <v>1</v>
       </c>
       <c r="H94" s="4">
-        <v>185</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E95" s="3">
         <f>(A95-D95)</f>
@@ -3201,19 +3201,19 @@
         <v>1</v>
       </c>
       <c r="H95" s="4">
-        <v>94</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E96" s="3">
         <f>(A96-D96)</f>
@@ -3226,19 +3226,19 @@
         <v>1</v>
       </c>
       <c r="H96" s="4">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E97" s="3">
         <f>(A97-D97)</f>
@@ -3251,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="H97" s="4">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E98" s="3">
         <f>(A98-D98)</f>
@@ -3276,19 +3276,19 @@
         <v>1</v>
       </c>
       <c r="H98" s="4">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E99" s="3">
         <f>(A99-D99)</f>
@@ -3301,23 +3301,23 @@
         <v>1</v>
       </c>
       <c r="H99" s="4">
-        <v>97</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E100" s="3">
         <f>(A100-D100)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F100" s="4">
         <v>1</v>
@@ -3326,23 +3326,23 @@
         <v>1</v>
       </c>
       <c r="H100" s="4">
-        <v>136</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E101" s="3">
         <f>(A101-D101)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F101" s="4">
         <v>1</v>
@@ -3351,23 +3351,23 @@
         <v>1</v>
       </c>
       <c r="H101" s="4">
-        <v>151</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E102" s="3">
         <f>(A102-D102)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F102" s="4">
         <v>1</v>
@@ -3381,18 +3381,18 @@
     </row>
     <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E103" s="3">
         <f>(A103-D103)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F103" s="4">
         <v>1</v>
@@ -3401,23 +3401,23 @@
         <v>1</v>
       </c>
       <c r="H103" s="4">
-        <v>168</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E104" s="3">
         <f>(A104-D104)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F104" s="4">
         <v>1</v>
@@ -3426,23 +3426,23 @@
         <v>1</v>
       </c>
       <c r="H104" s="4">
-        <v>172</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E105" s="3">
         <f>(A105-D105)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F105" s="4">
         <v>1</v>
@@ -3451,145 +3451,157 @@
         <v>1</v>
       </c>
       <c r="H105" s="4">
-        <v>163</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E106" s="3">
         <f>(A106-D106)</f>
-        <v>2</v>
-      </c>
-      <c r="F106" s="3">
-        <v>1</v>
-      </c>
-      <c r="G106" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="F106" s="4">
+        <v>1</v>
+      </c>
+      <c r="G106" s="4">
+        <v>1</v>
+      </c>
       <c r="H106" s="4">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="E107" s="3">
         <f>(A107-D107)</f>
-        <v>3</v>
-      </c>
-      <c r="F107" s="3">
-        <v>1</v>
-      </c>
-      <c r="G107" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="F107" s="4">
+        <v>1</v>
+      </c>
+      <c r="G107" s="4">
+        <v>1</v>
+      </c>
       <c r="H107" s="4">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="E108" s="3">
         <f>(A108-D108)</f>
-        <v>4</v>
-      </c>
-      <c r="F108" s="3">
-        <v>1</v>
-      </c>
-      <c r="G108" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="F108" s="4">
+        <v>1</v>
+      </c>
+      <c r="G108" s="4">
+        <v>1</v>
+      </c>
       <c r="H108" s="4">
-        <v>50</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="E109" s="3">
         <f>(A109-D109)</f>
-        <v>5</v>
-      </c>
-      <c r="F109" s="3">
-        <v>1</v>
-      </c>
-      <c r="G109" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F109" s="4">
+        <v>1</v>
+      </c>
+      <c r="G109" s="4">
+        <v>1</v>
+      </c>
       <c r="H109" s="4">
-        <v>117</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="E110" s="3">
         <f>(A110-D110)</f>
-        <v>5</v>
-      </c>
-      <c r="F110" s="3">
-        <v>1</v>
-      </c>
-      <c r="G110" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F110" s="4">
+        <v>1</v>
+      </c>
+      <c r="G110" s="4">
+        <v>1</v>
+      </c>
       <c r="H110" s="4">
-        <v>134</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E111" s="3">
         <f>(A111-D111)</f>
-        <v>5</v>
-      </c>
-      <c r="F111" s="3">
-        <v>1</v>
-      </c>
-      <c r="G111" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F111" s="4">
+        <v>1</v>
+      </c>
+      <c r="G111" s="4">
+        <v>1</v>
+      </c>
       <c r="H111" s="4">
-        <v>81</v>
+        <v>154</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3646,11 +3658,11 @@
       </c>
       <c r="G114" s="1">
         <f>SUM(G1:G112)</f>
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H114" s="1">
         <f>SUM(H1:H112)</f>
-        <v>13495</v>
+        <v>13486</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>